<commit_message>
Added large group of binding locations to the AR3... group of antibodies.
Because of this, some antibodies have very many locations (up to 25).

Had to change how column selector naming works.
</commit_message>
<xml_diff>
--- a/tabular/antibodyTable.xlsx
+++ b/tabular/antibodyTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15440" yWindow="1400" windowWidth="34580" windowHeight="22740"/>
+    <workbookView xWindow="9280" yWindow="1400" windowWidth="40540" windowHeight="26100" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Antibody table" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="200">
   <si>
     <t>Antibody</t>
   </si>
@@ -545,13 +545,97 @@
   </si>
   <si>
     <t>D206</t>
+  </si>
+  <si>
+    <t>BR10</t>
+  </si>
+  <si>
+    <t>BR11</t>
+  </si>
+  <si>
+    <t>BR20</t>
+  </si>
+  <si>
+    <t>BR21</t>
+  </si>
+  <si>
+    <t>BR12</t>
+  </si>
+  <si>
+    <t>BR13</t>
+  </si>
+  <si>
+    <t>BR14</t>
+  </si>
+  <si>
+    <t>BR15</t>
+  </si>
+  <si>
+    <t>BR17</t>
+  </si>
+  <si>
+    <t>BR18</t>
+  </si>
+  <si>
+    <t>BR19</t>
+  </si>
+  <si>
+    <t>BR22</t>
+  </si>
+  <si>
+    <t>C429</t>
+  </si>
+  <si>
+    <t>N430</t>
+  </si>
+  <si>
+    <t>S432</t>
+  </si>
+  <si>
+    <t>G440</t>
+  </si>
+  <si>
+    <t>C459</t>
+  </si>
+  <si>
+    <t>A499</t>
+  </si>
+  <si>
+    <t>C503</t>
+  </si>
+  <si>
+    <t>V515</t>
+  </si>
+  <si>
+    <t>G517</t>
+  </si>
+  <si>
+    <t>T518</t>
+  </si>
+  <si>
+    <t>D520</t>
+  </si>
+  <si>
+    <t>V536</t>
+  </si>
+  <si>
+    <t>T558</t>
+  </si>
+  <si>
+    <t>BR23</t>
+  </si>
+  <si>
+    <t>BR24</t>
+  </si>
+  <si>
+    <t>BR25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -581,6 +665,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -599,17 +699,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -912,10 +1029,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S55"/>
+  <dimension ref="A1:Z55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -923,7 +1040,7 @@
     <col min="2" max="10" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -954,17 +1071,56 @@
       <c r="J1" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K1" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -978,7 +1134,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -989,7 +1145,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>163</v>
       </c>
@@ -1000,7 +1156,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1017,7 +1173,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1034,7 +1190,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1045,7 +1201,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1059,7 +1215,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1076,7 +1232,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1093,7 +1249,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1107,7 +1263,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1121,7 +1277,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1132,7 +1288,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1146,7 +1302,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1163,7 +1319,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1180,7 +1336,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1203,75 +1359,279 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="22" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="O22" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="P22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="R22" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="S22" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="O23" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="P23" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q23" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="R23" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="S23" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="T23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="U23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V23" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="W23" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="X23" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="N24" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="O24" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="R24" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="S24" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C25" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M25" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N25" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="O25" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="P25" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q25" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="R25" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="S25" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="T25" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D22" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="U25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="V25" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F22" t="s">
+      <c r="W25" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="X25" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="Y25" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z25" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -1297,7 +1657,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>92</v>
       </c>
@@ -1314,7 +1674,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>164</v>
       </c>
@@ -1331,7 +1691,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -1342,7 +1702,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -2139,7 +2499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed error in column name.
</commit_message>
<xml_diff>
--- a/tabular/antibodyTable.xlsx
+++ b/tabular/antibodyTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9280" yWindow="1400" windowWidth="40540" windowHeight="26100" activeTab="2"/>
+    <workbookView xWindow="9280" yWindow="1400" windowWidth="40540" windowHeight="26100"/>
   </bookViews>
   <sheets>
     <sheet name="Antibody table" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="201">
   <si>
     <t>Antibody</t>
   </si>
@@ -629,6 +629,9 @@
   </si>
   <si>
     <t>BR25</t>
+  </si>
+  <si>
+    <t>BR16</t>
   </si>
 </sst>
 </file>
@@ -1031,8 +1034,8 @@
   </sheetPr>
   <dimension ref="A1:Z55"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1090,7 +1093,7 @@
         <v>179</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>179</v>
+        <v>200</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>180</v>
@@ -2499,7 +2502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated binding residues for HC84.20 and generated bindingMotifsReport.
</commit_message>
<xml_diff>
--- a/tabular/antibodyTable.xlsx
+++ b/tabular/antibodyTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9280" yWindow="1400" windowWidth="40540" windowHeight="26100"/>
+    <workbookView xWindow="3720" yWindow="1500" windowWidth="40540" windowHeight="26100"/>
   </bookViews>
   <sheets>
     <sheet name="Antibody table" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="201">
   <si>
     <t>Antibody</t>
   </si>
@@ -1035,7 +1035,7 @@
   <dimension ref="A1:Z55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1775,19 +1775,16 @@
       <c r="A37" t="s">
         <v>56</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C37" t="s">
         <v>40</v>
       </c>
-      <c r="C37" t="s">
-        <v>41</v>
-      </c>
       <c r="D37" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="E37" t="s">
-        <v>57</v>
-      </c>
-      <c r="F37" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update to HC-1 binding locations.
</commit_message>
<xml_diff>
--- a/tabular/antibodyTable.xlsx
+++ b/tabular/antibodyTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="1500" windowWidth="40540" windowHeight="26100"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="49860" windowHeight="28340"/>
   </bookViews>
   <sheets>
     <sheet name="Antibody table" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="201">
   <si>
     <t>Antibody</t>
   </si>
@@ -1035,7 +1035,7 @@
   <dimension ref="A1:Z55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1753,21 +1753,15 @@
         <v>65</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>184</v>
       </c>
       <c r="C35" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="D35" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="E35" t="s">
-        <v>16</v>
-      </c>
-      <c r="F35" t="s">
-        <v>17</v>
-      </c>
-      <c r="G35" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new antibody DAO1.
</commit_message>
<xml_diff>
--- a/tabular/antibodyTable.xlsx
+++ b/tabular/antibodyTable.xlsx
@@ -1,35 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28702"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshsinger/gitrepos_ssh/HCV-NABS/tabular/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="49860" windowHeight="28340"/>
+    <workbookView xWindow="4380" yWindow="1760" windowWidth="42860" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Antibody table" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Antibody table'!$A$34:$J$35</definedName>
+  </definedNames>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="206">
   <si>
     <t>Antibody</t>
   </si>
@@ -632,6 +630,21 @@
   </si>
   <si>
     <t>BR16</t>
+  </si>
+  <si>
+    <t>DAO1</t>
+  </si>
+  <si>
+    <t>G495</t>
+  </si>
+  <si>
+    <t>S512</t>
+  </si>
+  <si>
+    <t>L615</t>
+  </si>
+  <si>
+    <t>V636</t>
   </si>
 </sst>
 </file>
@@ -785,7 +798,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -820,7 +833,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -1032,18 +1045,18 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z55"/>
+  <dimension ref="A1:Z57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="M57" sqref="M57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="10" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1123,7 +1136,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1137,7 +1150,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1148,7 +1161,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26">
       <c r="A4" t="s">
         <v>163</v>
       </c>
@@ -1159,7 +1172,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1176,7 +1189,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1193,7 +1206,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1204,7 +1217,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1218,7 +1231,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1235,7 +1248,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1252,7 +1265,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1266,7 +1279,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1280,7 +1293,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1291,7 +1304,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1305,7 +1318,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1322,7 +1335,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1339,7 +1352,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1362,7 +1375,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" s="5" customFormat="1">
       <c r="A22" s="5" t="s">
         <v>43</v>
       </c>
@@ -1421,7 +1434,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" s="5" customFormat="1">
       <c r="A23" s="5" t="s">
         <v>48</v>
       </c>
@@ -1495,7 +1508,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" s="5" customFormat="1">
       <c r="A24" s="5" t="s">
         <v>49</v>
       </c>
@@ -1554,7 +1567,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" s="5" customFormat="1">
       <c r="A25" s="5" t="s">
         <v>50</v>
       </c>
@@ -1634,7 +1647,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -1660,7 +1673,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26">
       <c r="A29" t="s">
         <v>92</v>
       </c>
@@ -1677,7 +1690,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26">
       <c r="A30" t="s">
         <v>164</v>
       </c>
@@ -1694,7 +1707,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -1705,7 +1718,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -1716,7 +1729,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>60</v>
       </c>
@@ -1748,7 +1761,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -1765,7 +1778,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -1782,7 +1795,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -1799,7 +1812,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>165</v>
       </c>
@@ -1816,7 +1829,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
         <v>58</v>
       </c>
@@ -1830,7 +1843,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>59</v>
       </c>
@@ -1844,7 +1857,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
         <v>161</v>
       </c>
@@ -1861,7 +1874,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>68</v>
       </c>
@@ -1878,7 +1891,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10">
       <c r="A45" s="1" t="s">
         <v>71</v>
       </c>
@@ -1901,7 +1914,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
         <v>72</v>
       </c>
@@ -1924,7 +1937,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10">
       <c r="A47" t="s">
         <v>73</v>
       </c>
@@ -1938,7 +1951,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10">
       <c r="A48" t="s">
         <v>75</v>
       </c>
@@ -1949,7 +1962,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13">
       <c r="A50" t="s">
         <v>77</v>
       </c>
@@ -1969,7 +1982,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13">
       <c r="A52" t="s">
         <v>93</v>
       </c>
@@ -1995,7 +2008,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13">
       <c r="A53" t="s">
         <v>97</v>
       </c>
@@ -2018,7 +2031,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13">
       <c r="A55" t="s">
         <v>166</v>
       </c>
@@ -2050,9 +2063,56 @@
         <v>52</v>
       </c>
     </row>
+    <row r="57" spans="1:13">
+      <c r="A57" t="s">
+        <v>201</v>
+      </c>
+      <c r="B57" t="s">
+        <v>202</v>
+      </c>
+      <c r="C57" t="s">
+        <v>203</v>
+      </c>
+      <c r="D57" t="s">
+        <v>192</v>
+      </c>
+      <c r="E57" t="s">
+        <v>45</v>
+      </c>
+      <c r="F57" t="s">
+        <v>46</v>
+      </c>
+      <c r="G57" t="s">
+        <v>70</v>
+      </c>
+      <c r="H57" t="s">
+        <v>15</v>
+      </c>
+      <c r="I57" t="s">
+        <v>47</v>
+      </c>
+      <c r="J57" t="s">
+        <v>196</v>
+      </c>
+      <c r="K57" t="s">
+        <v>204</v>
+      </c>
+      <c r="L57" t="s">
+        <v>205</v>
+      </c>
+      <c r="M57" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A34:J35"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="54" orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2064,12 +2124,12 @@
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" s="3" t="s">
         <v>86</v>
       </c>
@@ -2077,7 +2137,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -2097,7 +2157,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2129,7 +2189,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>85</v>
       </c>
@@ -2149,7 +2209,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -2175,7 +2235,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>88</v>
       </c>
@@ -2183,7 +2243,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -2215,7 +2275,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>89</v>
       </c>
@@ -2247,7 +2307,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -2258,7 +2318,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>99</v>
       </c>
@@ -2275,12 +2335,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25" s="3" t="s">
         <v>86</v>
       </c>
@@ -2288,7 +2348,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>83</v>
       </c>
@@ -2308,7 +2368,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -2340,7 +2400,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -2360,7 +2420,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -2386,7 +2446,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>88</v>
       </c>
@@ -2394,7 +2454,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
         <v>67</v>
       </c>
@@ -2426,7 +2486,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -2455,7 +2515,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -2466,7 +2526,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
         <v>99</v>
       </c>
@@ -2485,7 +2545,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2497,9 +2562,9 @@
       <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:14">
       <c r="B2" s="3" t="s">
         <v>90</v>
       </c>
@@ -2507,7 +2572,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:14">
       <c r="B3" t="s">
         <v>32</v>
       </c>
@@ -2515,7 +2580,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:14">
       <c r="B4" t="s">
         <v>28</v>
       </c>
@@ -2526,7 +2591,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:14">
       <c r="B5" t="s">
         <v>22</v>
       </c>
@@ -2537,18 +2602,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:14">
       <c r="B6" t="s">
         <v>29</v>
       </c>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:14">
       <c r="B7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:14">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -2580,12 +2645,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:14">
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:14">
       <c r="B10" t="s">
         <v>4</v>
       </c>
@@ -2599,7 +2664,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:14">
       <c r="B11" t="s">
         <v>19</v>
       </c>
@@ -2607,7 +2672,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:14">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -2618,7 +2683,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:14">
       <c r="B13" t="s">
         <v>5</v>
       </c>
@@ -2638,7 +2703,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:14">
       <c r="B14" t="s">
         <v>6</v>
       </c>
@@ -2679,7 +2744,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:14">
       <c r="B15" t="s">
         <v>9</v>
       </c>
@@ -2687,12 +2752,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:14">
       <c r="B16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:13">
       <c r="B17" t="s">
         <v>44</v>
       </c>
@@ -2706,7 +2771,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13">
       <c r="B18" t="s">
         <v>63</v>
       </c>
@@ -2714,13 +2779,13 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13">
       <c r="B19" t="s">
         <v>64</v>
       </c>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13">
       <c r="B20" t="s">
         <v>38</v>
       </c>
@@ -2732,17 +2797,17 @@
       </c>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:13">
       <c r="B21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:13">
       <c r="B22" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:13">
       <c r="B23" t="s">
         <v>39</v>
       </c>
@@ -2759,7 +2824,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:13">
       <c r="B24" t="s">
         <v>61</v>
       </c>
@@ -2767,12 +2832,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:13">
       <c r="B25" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:13">
       <c r="B26" t="s">
         <v>40</v>
       </c>
@@ -2798,7 +2863,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:13">
       <c r="B27" t="s">
         <v>41</v>
       </c>
@@ -2830,7 +2895,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:13">
       <c r="B28" t="s">
         <v>42</v>
       </c>
@@ -2850,12 +2915,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:13">
       <c r="B29" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:13">
       <c r="B30" t="s">
         <v>45</v>
       </c>
@@ -2872,12 +2937,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:13">
       <c r="B31" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:13">
       <c r="B32" t="s">
         <v>46</v>
       </c>
@@ -2894,7 +2959,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:17">
       <c r="B33" t="s">
         <v>70</v>
       </c>
@@ -2902,7 +2967,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:17">
       <c r="B34" s="2" t="s">
         <v>15</v>
       </c>
@@ -2928,7 +2993,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:17">
       <c r="B35" t="s">
         <v>16</v>
       </c>
@@ -2963,7 +3028,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:17">
       <c r="B36" s="2" t="s">
         <v>17</v>
       </c>
@@ -3013,12 +3078,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:17">
       <c r="B37" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:17">
       <c r="B38" t="s">
         <v>47</v>
       </c>
@@ -3051,13 +3116,13 @@
       </c>
       <c r="M38" s="2"/>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:17">
       <c r="B39" t="s">
         <v>34</v>
       </c>
       <c r="M39" s="2"/>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:17">
       <c r="B40" t="s">
         <v>35</v>
       </c>
@@ -3075,31 +3140,31 @@
       </c>
       <c r="M40" s="2"/>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:17">
       <c r="B41" t="s">
         <v>81</v>
       </c>
       <c r="M41" s="2"/>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:17">
       <c r="B42" s="2" t="s">
         <v>78</v>
       </c>
       <c r="M42" s="2"/>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:17">
       <c r="B43" s="2" t="s">
         <v>79</v>
       </c>
       <c r="M43" s="2"/>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:17">
       <c r="B44" s="2" t="s">
         <v>80</v>
       </c>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:17">
       <c r="B45" s="2" t="s">
         <v>36</v>
       </c>
@@ -3110,12 +3175,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:17">
       <c r="B46" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:17">
       <c r="B47" t="s">
         <v>57</v>
       </c>
@@ -3123,7 +3188,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:17">
       <c r="B48" t="s">
         <v>52</v>
       </c>
@@ -3140,13 +3205,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:13">
       <c r="B49" t="s">
         <v>98</v>
       </c>
       <c r="M49" s="2"/>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:13">
       <c r="B50" t="s">
         <v>94</v>
       </c>
@@ -3154,17 +3219,22 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:13">
       <c r="B51" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:13">
       <c r="B52" t="s">
         <v>96</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates for the analysis of DAO1
</commit_message>
<xml_diff>
--- a/tabular/antibodyTable.xlsx
+++ b/tabular/antibodyTable.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28702"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshsinger/gitrepos_ssh/HCV-NABS/tabular/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="4380" yWindow="1760" windowWidth="42860" windowHeight="16060"/>
   </bookViews>
@@ -16,18 +21,18 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="207">
   <si>
     <t>Antibody</t>
   </si>
@@ -645,6 +650,9 @@
   </si>
   <si>
     <t>V636</t>
+  </si>
+  <si>
+    <t>DAO1_MINIMAL</t>
   </si>
 </sst>
 </file>
@@ -1045,18 +1053,18 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z57"/>
+  <dimension ref="A1:Z58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58:M58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="10" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1136,7 +1144,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1150,7 +1158,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1161,7 +1169,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>163</v>
       </c>
@@ -1172,7 +1180,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1189,7 +1197,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1206,7 +1214,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1217,7 +1225,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1231,7 +1239,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1248,7 +1256,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1265,7 +1273,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1279,7 +1287,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1293,7 +1301,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1304,7 +1312,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1318,7 +1326,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1335,7 +1343,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1352,7 +1360,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1375,7 +1383,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:26" s="5" customFormat="1">
+    <row r="22" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>43</v>
       </c>
@@ -1434,7 +1442,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:26" s="5" customFormat="1">
+    <row r="23" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>48</v>
       </c>
@@ -1508,7 +1516,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:26" s="5" customFormat="1">
+    <row r="24" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>49</v>
       </c>
@@ -1567,7 +1575,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:26" s="5" customFormat="1">
+    <row r="25" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>50</v>
       </c>
@@ -1647,7 +1655,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:26">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -1673,7 +1681,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:26">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>92</v>
       </c>
@@ -1690,7 +1698,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:26">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>164</v>
       </c>
@@ -1707,7 +1715,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:26">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -1718,7 +1726,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:26">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -1729,7 +1737,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>60</v>
       </c>
@@ -1761,7 +1769,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -1778,7 +1786,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -1795,7 +1803,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -1812,7 +1820,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>165</v>
       </c>
@@ -1829,7 +1837,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>58</v>
       </c>
@@ -1843,7 +1851,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>59</v>
       </c>
@@ -1857,7 +1865,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>161</v>
       </c>
@@ -1874,7 +1882,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>68</v>
       </c>
@@ -1891,7 +1899,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>71</v>
       </c>
@@ -1914,7 +1922,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>72</v>
       </c>
@@ -1937,7 +1945,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>73</v>
       </c>
@@ -1951,7 +1959,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>75</v>
       </c>
@@ -1962,7 +1970,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>77</v>
       </c>
@@ -1982,7 +1990,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>93</v>
       </c>
@@ -2008,7 +2016,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>97</v>
       </c>
@@ -2031,7 +2039,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>166</v>
       </c>
@@ -2063,7 +2071,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>201</v>
       </c>
@@ -2101,6 +2109,26 @@
         <v>205</v>
       </c>
       <c r="M57" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>206</v>
+      </c>
+      <c r="B58" t="s">
+        <v>203</v>
+      </c>
+      <c r="C58" t="s">
+        <v>45</v>
+      </c>
+      <c r="D58" t="s">
+        <v>46</v>
+      </c>
+      <c r="E58" t="s">
+        <v>205</v>
+      </c>
+      <c r="F58" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2108,11 +2136,6 @@
   <autoFilter ref="A34:J35"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" orientation="landscape"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2124,12 +2147,12 @@
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>86</v>
       </c>
@@ -2137,7 +2160,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -2157,7 +2180,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2189,7 +2212,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>85</v>
       </c>
@@ -2209,7 +2232,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -2235,7 +2258,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>88</v>
       </c>
@@ -2243,7 +2266,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -2275,7 +2298,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>89</v>
       </c>
@@ -2307,7 +2330,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -2318,7 +2341,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>99</v>
       </c>
@@ -2335,12 +2358,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>86</v>
       </c>
@@ -2348,7 +2371,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>83</v>
       </c>
@@ -2368,7 +2391,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -2400,7 +2423,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -2420,7 +2443,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -2446,7 +2469,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>88</v>
       </c>
@@ -2454,7 +2477,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>67</v>
       </c>
@@ -2486,7 +2509,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -2515,7 +2538,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -2526,7 +2549,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>99</v>
       </c>
@@ -2546,11 +2569,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2562,9 +2580,9 @@
       <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:14">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>90</v>
       </c>
@@ -2572,7 +2590,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="2:14">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>32</v>
       </c>
@@ -2580,7 +2598,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:14">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>28</v>
       </c>
@@ -2591,7 +2609,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:14">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>22</v>
       </c>
@@ -2602,18 +2620,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="2:14">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>29</v>
       </c>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="2:14">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:14">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -2645,12 +2663,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:14">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:14">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>4</v>
       </c>
@@ -2664,7 +2682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:14">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>19</v>
       </c>
@@ -2672,7 +2690,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:14">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -2683,7 +2701,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:14">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>5</v>
       </c>
@@ -2703,7 +2721,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:14">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>6</v>
       </c>
@@ -2744,7 +2762,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:14">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>9</v>
       </c>
@@ -2752,12 +2770,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="2:14">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:13">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>44</v>
       </c>
@@ -2771,7 +2789,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="2:13">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>63</v>
       </c>
@@ -2779,13 +2797,13 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="2:13">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>64</v>
       </c>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="2:13">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>38</v>
       </c>
@@ -2797,17 +2815,17 @@
       </c>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="2:13">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="2:13">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="2:13">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>39</v>
       </c>
@@ -2824,7 +2842,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="2:13">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>61</v>
       </c>
@@ -2832,12 +2850,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="2:13">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="2:13">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>40</v>
       </c>
@@ -2863,7 +2881,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="2:13">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>41</v>
       </c>
@@ -2895,7 +2913,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="2:13">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>42</v>
       </c>
@@ -2915,12 +2933,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="2:13">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="2:13">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>45</v>
       </c>
@@ -2937,12 +2955,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="2:13">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="2:13">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>46</v>
       </c>
@@ -2959,7 +2977,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="2:17">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>70</v>
       </c>
@@ -2967,7 +2985,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="2:17">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
         <v>15</v>
       </c>
@@ -2993,7 +3011,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="2:17">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>16</v>
       </c>
@@ -3028,7 +3046,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="2:17">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>17</v>
       </c>
@@ -3078,12 +3096,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="2:17">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="2:17">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>47</v>
       </c>
@@ -3116,13 +3134,13 @@
       </c>
       <c r="M38" s="2"/>
     </row>
-    <row r="39" spans="2:17">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>34</v>
       </c>
       <c r="M39" s="2"/>
     </row>
-    <row r="40" spans="2:17">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>35</v>
       </c>
@@ -3140,31 +3158,31 @@
       </c>
       <c r="M40" s="2"/>
     </row>
-    <row r="41" spans="2:17">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>81</v>
       </c>
       <c r="M41" s="2"/>
     </row>
-    <row r="42" spans="2:17">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>78</v>
       </c>
       <c r="M42" s="2"/>
     </row>
-    <row r="43" spans="2:17">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
         <v>79</v>
       </c>
       <c r="M43" s="2"/>
     </row>
-    <row r="44" spans="2:17">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
         <v>80</v>
       </c>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="2:17">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
         <v>36</v>
       </c>
@@ -3175,12 +3193,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="2:17">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="2:17">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>57</v>
       </c>
@@ -3188,7 +3206,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="2:17">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>52</v>
       </c>
@@ -3205,13 +3223,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="2:13">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>98</v>
       </c>
       <c r="M49" s="2"/>
     </row>
-    <row r="50" spans="2:13">
+    <row r="50" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>94</v>
       </c>
@@ -3219,22 +3237,17 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="2:13">
+    <row r="51" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="2:13">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>96</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>